<commit_message>
add row count logic to scan
</commit_message>
<xml_diff>
--- a/reports/table_actions_report.xlsx
+++ b/reports/table_actions_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,63 +449,82 @@
           <t>HasAccountId</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>RowCount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>[dbo].[EntityRole]</t>
+          <t>[dbo].[Users]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t>DELETE FILTERED</t>
+        </is>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[dbo].[Logs]</t>
+          <t>[dbo].[Orders]</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TRUNCATED</t>
+          <t>DELETE FILTERED</t>
         </is>
       </c>
       <c r="C3" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>[dbo].[Orders]</t>
+          <t>[dbo].[Logs]</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>DELETE WHERE AccountId &lt;&gt; 8 OR IS NULL</t>
+          <t>TRUNCATED</t>
         </is>
       </c>
       <c r="C4" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>[dbo].[Users]</t>
+          <t>[dbo].[EntityRole]</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DELETE WHERE AccountId &lt;&gt; 8 OR IS NULL</t>
+          <t>TRUNCATED</t>
         </is>
       </c>
       <c r="C5" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>